<commit_message>
Work on xlsx export
</commit_message>
<xml_diff>
--- a/EnergTemplate.xlsx
+++ b/EnergTemplate.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MafuraG\Documents\GitHub\enegpassport\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="19440" windowHeight="11055"/>
   </bookViews>
@@ -6189,7 +6194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -6365,17 +6370,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6384,10 +6380,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6404,11 +6403,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6420,6 +6428,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -6468,7 +6479,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6503,7 +6514,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6714,8 +6725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72:D72"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6745,16 +6756,16 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -6803,20 +6814,20 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="3"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="74" t="s">
         <v>134</v>
       </c>
       <c r="H6" s="16"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="71"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -6831,10 +6842,10 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="17"/>
@@ -6843,18 +6854,18 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
@@ -6870,14 +6881,14 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63" t="s">
+      <c r="C11" s="72"/>
+      <c r="D11" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="E11" s="63"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="6" t="s">
         <v>136</v>
       </c>
@@ -6889,25 +6900,25 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="64"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -6917,12 +6928,12 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -6932,16 +6943,16 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="63"/>
+      <c r="C15" s="60"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="65" t="s">
+      <c r="E15" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
       <c r="H15" s="6" t="s">
         <v>137</v>
       </c>
@@ -6951,13 +6962,13 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="18"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -6966,26 +6977,26 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
@@ -6994,12 +7005,12 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="5"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -7007,18 +7018,18 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
@@ -7037,44 +7048,44 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
     </row>
     <row r="24" spans="1:10" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
     </row>
@@ -7097,28 +7108,28 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="60" t="s">
+      <c r="A26" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -7137,18 +7148,18 @@
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
@@ -7175,18 +7186,18 @@
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="66"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
@@ -7349,18 +7360,18 @@
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="60" t="s">
+      <c r="A41" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="60"/>
-      <c r="J41" s="60"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="62"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
@@ -7453,28 +7464,28 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="66"/>
-      <c r="C47" s="66"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="66"/>
-      <c r="F47" s="66"/>
-      <c r="G47" s="66"/>
-      <c r="H47" s="66"/>
-      <c r="I47" s="66"/>
-      <c r="J47" s="66"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="63"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="60"/>
+      <c r="F48" s="60"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -7485,13 +7496,13 @@
       <c r="B49" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C49" s="63" t="s">
+      <c r="C49" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
       <c r="H49" s="3" t="s">
         <v>157</v>
       </c>
@@ -7513,15 +7524,15 @@
       <c r="J50" s="3"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="69" t="s">
+      <c r="A51" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="69"/>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
-      <c r="E51" s="69"/>
-      <c r="F51" s="69"/>
-      <c r="G51" s="69"/>
+      <c r="B51" s="67"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="67"/>
       <c r="H51" s="12" t="s">
         <v>61</v>
       </c>
@@ -7531,10 +7542,10 @@
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="7"/>
-      <c r="C52" s="63" t="s">
+      <c r="C52" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="70"/>
+      <c r="D52" s="68"/>
       <c r="E52" s="9"/>
       <c r="F52" s="34" t="s">
         <v>62</v>
@@ -7547,13 +7558,13 @@
       <c r="J52" s="7"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="64" t="s">
+      <c r="A53" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="64"/>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
       <c r="F53" s="36" t="s">
         <v>64</v>
       </c>
@@ -7571,27 +7582,27 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="69" t="s">
+      <c r="A54" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="69"/>
-      <c r="C54" s="69"/>
-      <c r="D54" s="69"/>
-      <c r="E54" s="69"/>
-      <c r="F54" s="69"/>
+      <c r="B54" s="67"/>
+      <c r="C54" s="67"/>
+      <c r="D54" s="67"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="67"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
     </row>
     <row r="55" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="63" t="s">
+      <c r="A55" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="63"/>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="70"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="68"/>
       <c r="F55" s="34" t="s">
         <v>68</v>
       </c>
@@ -7603,26 +7614,26 @@
       <c r="J55" s="9"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="69" t="s">
+      <c r="A56" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="B56" s="69"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
+      <c r="B56" s="67"/>
+      <c r="C56" s="67"/>
+      <c r="D56" s="67"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="67"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
     </row>
     <row r="57" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="63" t="s">
+      <c r="A57" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="63"/>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
       <c r="E57" s="5"/>
       <c r="F57" s="37" t="s">
         <v>71</v>
@@ -7649,10 +7660,10 @@
       <c r="J58" s="9"/>
     </row>
     <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="71" t="s">
+      <c r="A59" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="71"/>
+      <c r="B59" s="69"/>
       <c r="C59" s="39" t="s">
         <v>164</v>
       </c>
@@ -7679,11 +7690,11 @@
       <c r="J60" s="7"/>
     </row>
     <row r="61" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="67" t="s">
+      <c r="A61" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="B61" s="68"/>
-      <c r="C61" s="68"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
       <c r="D61" s="40" t="s">
         <v>76</v>
       </c>
@@ -7729,10 +7740,10 @@
       <c r="B64" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="63" t="s">
+      <c r="C64" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="D64" s="63"/>
+      <c r="D64" s="60"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -7741,18 +7752,18 @@
       <c r="J64" s="7"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="60"/>
-      <c r="C65" s="60"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
-      <c r="F65" s="60"/>
-      <c r="G65" s="60"/>
-      <c r="H65" s="60"/>
-      <c r="I65" s="60"/>
-      <c r="J65" s="60"/>
+      <c r="B65" s="62"/>
+      <c r="C65" s="62"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="62"/>
+      <c r="I65" s="62"/>
+      <c r="J65" s="62"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="44"/>
@@ -7771,18 +7782,18 @@
       <c r="J66" s="44"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="66" t="s">
+      <c r="A67" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B67" s="66"/>
-      <c r="C67" s="66"/>
-      <c r="D67" s="66"/>
-      <c r="E67" s="66"/>
-      <c r="F67" s="66"/>
-      <c r="G67" s="66"/>
-      <c r="H67" s="66"/>
-      <c r="I67" s="66"/>
-      <c r="J67" s="66"/>
+      <c r="B67" s="63"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="63"/>
+      <c r="H67" s="63"/>
+      <c r="I67" s="63"/>
+      <c r="J67" s="63"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
@@ -7801,18 +7812,18 @@
       <c r="J68" s="7"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="60"/>
-      <c r="C69" s="60"/>
-      <c r="D69" s="60"/>
-      <c r="E69" s="60"/>
-      <c r="F69" s="60"/>
-      <c r="G69" s="60"/>
-      <c r="H69" s="60"/>
-      <c r="I69" s="60"/>
-      <c r="J69" s="60"/>
+      <c r="B69" s="62"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="62"/>
+      <c r="G69" s="62"/>
+      <c r="H69" s="62"/>
+      <c r="I69" s="62"/>
+      <c r="J69" s="62"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
@@ -7847,10 +7858,10 @@
       <c r="B72" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C72" s="63" t="s">
+      <c r="C72" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="D72" s="63"/>
+      <c r="D72" s="60"/>
       <c r="E72" s="9"/>
       <c r="F72" s="46" t="s">
         <v>79</v>
@@ -7901,11 +7912,11 @@
       <c r="J75" s="44"/>
     </row>
     <row r="76" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="72" t="s">
+      <c r="A76" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="B76" s="72"/>
-      <c r="C76" s="72"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="64"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
       <c r="F76" s="49" t="s">
@@ -7931,18 +7942,18 @@
       <c r="J77" s="9"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="60" t="s">
+      <c r="A78" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="B78" s="60"/>
-      <c r="C78" s="60"/>
-      <c r="D78" s="60"/>
-      <c r="E78" s="60"/>
-      <c r="F78" s="60"/>
-      <c r="G78" s="60"/>
-      <c r="H78" s="60"/>
-      <c r="I78" s="60"/>
-      <c r="J78" s="60"/>
+      <c r="B78" s="62"/>
+      <c r="C78" s="62"/>
+      <c r="D78" s="62"/>
+      <c r="E78" s="62"/>
+      <c r="F78" s="62"/>
+      <c r="G78" s="62"/>
+      <c r="H78" s="62"/>
+      <c r="I78" s="62"/>
+      <c r="J78" s="62"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="9"/>
@@ -7957,32 +7968,32 @@
       <c r="J79" s="9"/>
     </row>
     <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="63" t="s">
+      <c r="A80" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B80" s="63"/>
-      <c r="C80" s="63"/>
-      <c r="D80" s="63"/>
-      <c r="E80" s="63"/>
-      <c r="F80" s="63"/>
+      <c r="B80" s="60"/>
+      <c r="C80" s="60"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="60"/>
+      <c r="F80" s="60"/>
       <c r="G80" s="6"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="60" t="s">
+      <c r="A81" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="B81" s="60"/>
-      <c r="C81" s="60"/>
-      <c r="D81" s="60"/>
-      <c r="E81" s="60"/>
-      <c r="F81" s="60"/>
-      <c r="G81" s="60"/>
-      <c r="H81" s="60"/>
-      <c r="I81" s="60"/>
-      <c r="J81" s="60"/>
+      <c r="B81" s="62"/>
+      <c r="C81" s="62"/>
+      <c r="D81" s="62"/>
+      <c r="E81" s="62"/>
+      <c r="F81" s="62"/>
+      <c r="G81" s="62"/>
+      <c r="H81" s="62"/>
+      <c r="I81" s="62"/>
+      <c r="J81" s="62"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
@@ -8005,18 +8016,18 @@
       <c r="J82" s="9"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="60" t="s">
+      <c r="A83" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="B83" s="60"/>
-      <c r="C83" s="60"/>
-      <c r="D83" s="60"/>
-      <c r="E83" s="60"/>
-      <c r="F83" s="60"/>
-      <c r="G83" s="60"/>
-      <c r="H83" s="60"/>
-      <c r="I83" s="60"/>
-      <c r="J83" s="60"/>
+      <c r="B83" s="62"/>
+      <c r="C83" s="62"/>
+      <c r="D83" s="62"/>
+      <c r="E83" s="62"/>
+      <c r="F83" s="62"/>
+      <c r="G83" s="62"/>
+      <c r="H83" s="62"/>
+      <c r="I83" s="62"/>
+      <c r="J83" s="62"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="9"/>
@@ -8039,18 +8050,18 @@
       <c r="J84" s="9"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="60" t="s">
+      <c r="A85" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B85" s="60"/>
-      <c r="C85" s="60"/>
-      <c r="D85" s="60"/>
-      <c r="E85" s="60"/>
-      <c r="F85" s="60"/>
-      <c r="G85" s="60"/>
-      <c r="H85" s="60"/>
-      <c r="I85" s="60"/>
-      <c r="J85" s="60"/>
+      <c r="B85" s="62"/>
+      <c r="C85" s="62"/>
+      <c r="D85" s="62"/>
+      <c r="E85" s="62"/>
+      <c r="F85" s="62"/>
+      <c r="G85" s="62"/>
+      <c r="H85" s="62"/>
+      <c r="I85" s="62"/>
+      <c r="J85" s="62"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="9"/>
@@ -8121,12 +8132,12 @@
       <c r="J88" s="9"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="63" t="s">
+      <c r="A89" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="B89" s="63"/>
-      <c r="C89" s="63"/>
-      <c r="D89" s="63"/>
+      <c r="B89" s="60"/>
+      <c r="C89" s="60"/>
+      <c r="D89" s="60"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
@@ -8135,18 +8146,18 @@
       <c r="J89" s="7"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="60" t="s">
+      <c r="A90" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B90" s="60"/>
-      <c r="C90" s="60"/>
-      <c r="D90" s="60"/>
-      <c r="E90" s="60"/>
-      <c r="F90" s="60"/>
-      <c r="G90" s="60"/>
-      <c r="H90" s="60"/>
-      <c r="I90" s="60"/>
-      <c r="J90" s="60"/>
+      <c r="B90" s="62"/>
+      <c r="C90" s="62"/>
+      <c r="D90" s="62"/>
+      <c r="E90" s="62"/>
+      <c r="F90" s="62"/>
+      <c r="G90" s="62"/>
+      <c r="H90" s="62"/>
+      <c r="I90" s="62"/>
+      <c r="J90" s="62"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
@@ -8205,18 +8216,18 @@
       <c r="J92" s="9"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="60" t="s">
+      <c r="A93" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="B93" s="60"/>
-      <c r="C93" s="60"/>
-      <c r="D93" s="60"/>
-      <c r="E93" s="60"/>
-      <c r="F93" s="60"/>
-      <c r="G93" s="60"/>
-      <c r="H93" s="60"/>
-      <c r="I93" s="60"/>
-      <c r="J93" s="60"/>
+      <c r="B93" s="62"/>
+      <c r="C93" s="62"/>
+      <c r="D93" s="62"/>
+      <c r="E93" s="62"/>
+      <c r="F93" s="62"/>
+      <c r="G93" s="62"/>
+      <c r="H93" s="62"/>
+      <c r="I93" s="62"/>
+      <c r="J93" s="62"/>
     </row>
     <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="7"/>
@@ -8275,13 +8286,13 @@
       <c r="J97" s="9"/>
     </row>
     <row r="98" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="64" t="s">
+      <c r="A98" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="B98" s="64"/>
-      <c r="C98" s="64"/>
-      <c r="D98" s="64"/>
-      <c r="E98" s="64"/>
+      <c r="B98" s="61"/>
+      <c r="C98" s="61"/>
+      <c r="D98" s="61"/>
+      <c r="E98" s="61"/>
       <c r="F98" s="8"/>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
@@ -8317,16 +8328,16 @@
       <c r="J100" s="9"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="73" t="s">
+      <c r="A101" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="B101" s="73"/>
-      <c r="C101" s="73"/>
-      <c r="D101" s="73"/>
-      <c r="E101" s="73"/>
-      <c r="F101" s="73"/>
-      <c r="G101" s="73"/>
-      <c r="H101" s="73"/>
+      <c r="B101" s="59"/>
+      <c r="C101" s="59"/>
+      <c r="D101" s="59"/>
+      <c r="E101" s="59"/>
+      <c r="F101" s="59"/>
+      <c r="G101" s="59"/>
+      <c r="H101" s="59"/>
       <c r="I101" s="9"/>
       <c r="J101" s="9"/>
     </row>
@@ -8343,11 +8354,11 @@
       <c r="J102" s="9"/>
     </row>
     <row r="103" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="63" t="s">
+      <c r="A103" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="B103" s="63"/>
-      <c r="C103" s="63"/>
+      <c r="B103" s="60"/>
+      <c r="C103" s="60"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
@@ -8387,13 +8398,13 @@
       <c r="J105" s="7"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="73" t="s">
+      <c r="A106" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="B106" s="73"/>
-      <c r="C106" s="73"/>
-      <c r="D106" s="73"/>
-      <c r="E106" s="73"/>
+      <c r="B106" s="59"/>
+      <c r="C106" s="59"/>
+      <c r="D106" s="59"/>
+      <c r="E106" s="59"/>
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
@@ -8401,12 +8412,12 @@
       <c r="J106" s="7"/>
     </row>
     <row r="107" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="63" t="s">
+      <c r="A107" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="B107" s="63"/>
-      <c r="C107" s="63"/>
-      <c r="D107" s="63"/>
+      <c r="B107" s="60"/>
+      <c r="C107" s="60"/>
+      <c r="D107" s="60"/>
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
       <c r="G107" s="9"/>
@@ -8445,17 +8456,17 @@
       <c r="J109" s="9"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="73" t="s">
+      <c r="A110" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="B110" s="73"/>
-      <c r="C110" s="73"/>
-      <c r="D110" s="73"/>
-      <c r="E110" s="73"/>
-      <c r="F110" s="73"/>
-      <c r="G110" s="73"/>
-      <c r="H110" s="73"/>
-      <c r="I110" s="73"/>
+      <c r="B110" s="59"/>
+      <c r="C110" s="59"/>
+      <c r="D110" s="59"/>
+      <c r="E110" s="59"/>
+      <c r="F110" s="59"/>
+      <c r="G110" s="59"/>
+      <c r="H110" s="59"/>
+      <c r="I110" s="59"/>
       <c r="J110" s="9"/>
     </row>
     <row r="111" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8471,10 +8482,10 @@
       <c r="J111" s="9"/>
     </row>
     <row r="112" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="64" t="s">
+      <c r="A112" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="B112" s="64"/>
+      <c r="B112" s="61"/>
       <c r="C112" s="37" t="s">
         <v>132</v>
       </c>
@@ -8504,51 +8515,6 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A106:E106"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A110:I110"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A90:J90"/>
-    <mergeCell ref="A93:J93"/>
-    <mergeCell ref="A98:E98"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="A103:C103"/>
-    <mergeCell ref="A85:J85"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="A67:J67"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A78:J78"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="A83:J83"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A47:J47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A22:J22"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A31:J31"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A6:D6"/>
@@ -8562,6 +8528,51 @@
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A47:J47"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A85:J85"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="A67:J67"/>
+    <mergeCell ref="A69:J69"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A78:J78"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="A83:J83"/>
+    <mergeCell ref="A106:E106"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A110:I110"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A90:J90"/>
+    <mergeCell ref="A93:J93"/>
+    <mergeCell ref="A98:E98"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="A103:C103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Excel Template has been slightly modified
</commit_message>
<xml_diff>
--- a/EnergTemplate.xlsx
+++ b/EnergTemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="204">
   <si>
     <t>1. Удельная вентиляционная характеристика здания</t>
   </si>
@@ -6175,6 +6175,52 @@
   </si>
   <si>
     <t>val-64</t>
+  </si>
+  <si>
+    <r>
+      <t>А - площадь А</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>ж</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> для жилых помещений, А</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>р</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> - для общественных зданий.</t>
+    </r>
+  </si>
+  <si>
+    <t>val-65</t>
   </si>
 </sst>
 </file>
@@ -6465,7 +6511,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -6581,9 +6627,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -6696,15 +6739,28 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -7011,10 +7067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7044,16 +7100,16 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -7102,20 +7158,20 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
       <c r="E6" s="3"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="58" t="s">
         <v>130</v>
       </c>
       <c r="H6" s="16"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="62"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="61"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -7130,10 +7186,10 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="17"/>
@@ -7142,18 +7198,18 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
@@ -7169,14 +7225,14 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64" t="s">
+      <c r="C11" s="62"/>
+      <c r="D11" s="63" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="64"/>
+      <c r="E11" s="63"/>
       <c r="F11" s="6" t="s">
         <v>132</v>
       </c>
@@ -7188,25 +7244,25 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -7216,12 +7272,12 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -7231,16 +7287,16 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="64"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
       <c r="H15" s="6" t="s">
         <v>133</v>
       </c>
@@ -7250,13 +7306,13 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
       <c r="F16" s="18"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -7265,26 +7321,26 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
@@ -7293,12 +7349,12 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
       <c r="F19" s="5"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -7306,18 +7362,18 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
@@ -7336,44 +7392,44 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="60" t="s">
         <v>192</v>
       </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
     </row>
     <row r="24" spans="1:10" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="60" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
     </row>
@@ -7382,7 +7438,7 @@
       <c r="B25" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="56" t="s">
         <v>135</v>
       </c>
       <c r="D25" s="20" t="s">
@@ -7396,28 +7452,28 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="64" t="s">
+      <c r="B27" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -7436,18 +7492,18 @@
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="61" t="s">
+      <c r="A29" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
@@ -7474,18 +7530,18 @@
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
@@ -7648,18 +7704,18 @@
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="61" t="s">
+      <c r="A41" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="61"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="61"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
@@ -7752,28 +7808,28 @@
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="67" t="s">
+      <c r="A47" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="67"/>
-      <c r="C47" s="67"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="67"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="67"/>
-      <c r="I47" s="67"/>
-      <c r="J47" s="67"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="66"/>
+      <c r="H47" s="66"/>
+      <c r="I47" s="66"/>
+      <c r="J47" s="66"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="64" t="s">
+      <c r="B48" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -7784,13 +7840,13 @@
       <c r="B49" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C49" s="64" t="s">
+      <c r="C49" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
       <c r="H49" s="3" t="s">
         <v>153</v>
       </c>
@@ -7812,15 +7868,15 @@
       <c r="J50" s="3"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="70" t="s">
+      <c r="A51" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="70"/>
-      <c r="C51" s="70"/>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
+      <c r="B51" s="69"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
       <c r="H51" s="12" t="s">
         <v>59</v>
       </c>
@@ -7830,10 +7886,10 @@
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="7"/>
-      <c r="C52" s="64" t="s">
+      <c r="C52" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="D52" s="71"/>
+      <c r="D52" s="70"/>
       <c r="E52" s="9"/>
       <c r="F52" s="34" t="s">
         <v>60</v>
@@ -7846,13 +7902,13 @@
       <c r="J52" s="7"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="65" t="s">
+      <c r="A53" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="65"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="65"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="64"/>
       <c r="F53" s="36" t="s">
         <v>62</v>
       </c>
@@ -7870,27 +7926,27 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="70" t="s">
+      <c r="A54" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="70"/>
-      <c r="C54" s="70"/>
-      <c r="D54" s="70"/>
-      <c r="E54" s="70"/>
-      <c r="F54" s="70"/>
+      <c r="B54" s="69"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="69"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
     </row>
     <row r="55" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="64" t="s">
+      <c r="A55" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="B55" s="64"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="64"/>
-      <c r="E55" s="71"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="70"/>
       <c r="F55" s="34" t="s">
         <v>65</v>
       </c>
@@ -7902,26 +7958,26 @@
       <c r="J55" s="9"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="70" t="s">
+      <c r="A56" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="70"/>
-      <c r="C56" s="70"/>
-      <c r="D56" s="70"/>
-      <c r="E56" s="70"/>
-      <c r="F56" s="70"/>
+      <c r="B56" s="69"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
+      <c r="F56" s="69"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
     </row>
     <row r="57" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="64" t="s">
+      <c r="A57" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="B57" s="64"/>
-      <c r="C57" s="64"/>
-      <c r="D57" s="64"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="63"/>
       <c r="E57" s="5"/>
       <c r="F57" s="37" t="s">
         <v>67</v>
@@ -7940,37 +7996,37 @@
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
-      <c r="E58" s="75" t="s">
+      <c r="E58" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
-      <c r="I58" s="75"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="74"/>
       <c r="J58" s="9"/>
     </row>
     <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="72" t="s">
+      <c r="A59" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="72"/>
-      <c r="C59" s="39" t="s">
+      <c r="B59" s="71"/>
+      <c r="C59" s="84" t="s">
         <v>160</v>
       </c>
       <c r="D59" s="9"/>
-      <c r="E59" s="76" t="s">
+      <c r="E59" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="F59" s="77" t="s">
+      <c r="F59" s="83" t="s">
         <v>200</v>
       </c>
-      <c r="G59" s="78" t="s">
+      <c r="G59" s="76" t="s">
         <v>199</v>
       </c>
-      <c r="H59" s="79" t="s">
+      <c r="H59" s="77" t="s">
         <v>201</v>
       </c>
-      <c r="I59" s="80"/>
+      <c r="I59" s="78"/>
       <c r="J59" s="9"/>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7988,18 +8044,18 @@
       <c r="J60" s="7"/>
     </row>
     <row r="61" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="68" t="s">
+      <c r="A61" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="B61" s="69"/>
-      <c r="C61" s="69"/>
-      <c r="D61" s="40" t="s">
+      <c r="B61" s="68"/>
+      <c r="C61" s="68"/>
+      <c r="D61" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E61" s="41" t="s">
+      <c r="E61" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="F61" s="58" t="s">
+      <c r="F61" s="57" t="s">
         <v>73</v>
       </c>
       <c r="G61" s="7"/>
@@ -8009,10 +8065,10 @@
     </row>
     <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
+      <c r="B62" s="41"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
       <c r="F62" s="7"/>
       <c r="G62" s="9"/>
       <c r="H62" s="7"/>
@@ -8038,10 +8094,10 @@
       <c r="B64" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C64" s="64" t="s">
+      <c r="C64" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="D64" s="64"/>
+      <c r="D64" s="63"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -8049,573 +8105,578 @@
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="61" t="s">
+    <row r="65" spans="1:11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="79"/>
+      <c r="B65" s="80" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" s="80"/>
+      <c r="D65" s="80"/>
+      <c r="E65" s="80"/>
+      <c r="F65" s="80"/>
+      <c r="G65" s="80"/>
+      <c r="H65" s="81" t="s">
+        <v>203</v>
+      </c>
+      <c r="I65" s="78"/>
+      <c r="J65" s="78"/>
+      <c r="K65" s="82"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="61"/>
-      <c r="C65" s="61"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="61"/>
-      <c r="G65" s="61"/>
-      <c r="H65" s="61"/>
-      <c r="I65" s="61"/>
-      <c r="J65" s="61"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
-      <c r="B66" s="45" t="s">
+      <c r="B66" s="60"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="60"/>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="60"/>
+      <c r="I66" s="60"/>
+      <c r="J66" s="60"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="43"/>
+      <c r="B67" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D66" s="44"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="44"/>
-      <c r="I66" s="44"/>
-      <c r="J66" s="44"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="67" t="s">
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="43"/>
+      <c r="I67" s="43"/>
+      <c r="J67" s="43"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="67"/>
-      <c r="C67" s="67"/>
-      <c r="D67" s="67"/>
-      <c r="E67" s="67"/>
-      <c r="F67" s="67"/>
-      <c r="G67" s="67"/>
-      <c r="H67" s="67"/>
-      <c r="I67" s="67"/>
-      <c r="J67" s="67"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="66"/>
+      <c r="C68" s="66"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="66"/>
+      <c r="H68" s="66"/>
+      <c r="I68" s="66"/>
+      <c r="J68" s="66"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="61" t="s">
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="B69" s="61"/>
-      <c r="C69" s="61"/>
-      <c r="D69" s="61"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="61"/>
-      <c r="G69" s="61"/>
-      <c r="H69" s="61"/>
-      <c r="I69" s="61"/>
-      <c r="J69" s="61"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="60"/>
+      <c r="C70" s="60"/>
+      <c r="D70" s="60"/>
+      <c r="E70" s="60"/>
+      <c r="F70" s="60"/>
+      <c r="G70" s="60"/>
+      <c r="H70" s="60"/>
+      <c r="I70" s="60"/>
+      <c r="J70" s="60"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
-      <c r="B71" s="44"/>
-      <c r="C71" s="44"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="9"/>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="9"/>
+      <c r="B73" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C72" s="64" t="s">
+      <c r="C73" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="D72" s="64"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="46" t="s">
+      <c r="D73" s="63"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G72" s="47" t="s">
+      <c r="G73" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="48" t="s">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="B74" s="48"/>
-      <c r="C74" s="48"/>
-      <c r="D74" s="48"/>
-      <c r="E74" s="48"/>
-      <c r="F74" s="48"/>
-      <c r="G74" s="48"/>
-      <c r="H74" s="44"/>
-      <c r="I74" s="44"/>
-      <c r="J74" s="44"/>
-    </row>
-    <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="44"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="44"/>
-      <c r="G75" s="44"/>
-      <c r="H75" s="44"/>
-      <c r="I75" s="44"/>
-      <c r="J75" s="44"/>
-    </row>
-    <row r="76" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="73" t="s">
+      <c r="B75" s="47"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="43"/>
+      <c r="J75" s="43"/>
+    </row>
+    <row r="76" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="43"/>
+      <c r="F76" s="43"/>
+      <c r="G76" s="43"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="43"/>
+      <c r="J76" s="43"/>
+    </row>
+    <row r="77" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="73"/>
-      <c r="C76" s="73"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="G76" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="H76" s="44"/>
-      <c r="I76" s="44"/>
-      <c r="J76" s="44"/>
-    </row>
-    <row r="77" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9"/>
+      <c r="B77" s="72"/>
+      <c r="C77" s="72"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="61" t="s">
+      <c r="F77" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G77" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="H77" s="43"/>
+      <c r="I77" s="43"/>
+      <c r="J77" s="43"/>
+    </row>
+    <row r="78" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="B78" s="61"/>
-      <c r="C78" s="61"/>
-      <c r="D78" s="61"/>
-      <c r="E78" s="61"/>
-      <c r="F78" s="61"/>
-      <c r="G78" s="61"/>
-      <c r="H78" s="61"/>
-      <c r="I78" s="61"/>
-      <c r="J78" s="61"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="9"/>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
-      <c r="J79" s="9"/>
-    </row>
-    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="64" t="s">
+      <c r="B79" s="60"/>
+      <c r="C79" s="60"/>
+      <c r="D79" s="60"/>
+      <c r="E79" s="60"/>
+      <c r="F79" s="60"/>
+      <c r="G79" s="60"/>
+      <c r="H79" s="60"/>
+      <c r="I79" s="60"/>
+      <c r="J79" s="60"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+    </row>
+    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="B80" s="64"/>
-      <c r="C80" s="64"/>
-      <c r="D80" s="64"/>
-      <c r="E80" s="64"/>
-      <c r="F80" s="64"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="7"/>
-      <c r="I80" s="7"/>
-      <c r="J80" s="7"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="61" t="s">
+      <c r="B81" s="63"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="63"/>
+      <c r="E81" s="63"/>
+      <c r="F81" s="63"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="B81" s="61"/>
-      <c r="C81" s="61"/>
-      <c r="D81" s="61"/>
-      <c r="E81" s="61"/>
-      <c r="F81" s="61"/>
-      <c r="G81" s="61"/>
-      <c r="H81" s="61"/>
-      <c r="I81" s="61"/>
-      <c r="J81" s="61"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="60"/>
+      <c r="C82" s="60"/>
+      <c r="D82" s="60"/>
+      <c r="E82" s="60"/>
+      <c r="F82" s="60"/>
+      <c r="G82" s="60"/>
+      <c r="H82" s="60"/>
+      <c r="I82" s="60"/>
+      <c r="J82" s="60"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="9"/>
+      <c r="B83" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E83" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="9"/>
-      <c r="J82" s="9"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="61" t="s">
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="9"/>
+      <c r="J83" s="9"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="61"/>
-      <c r="C83" s="61"/>
-      <c r="D83" s="61"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="61"/>
-      <c r="G83" s="61"/>
-      <c r="H83" s="61"/>
-      <c r="I83" s="61"/>
-      <c r="J83" s="61"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="60"/>
+      <c r="C84" s="60"/>
+      <c r="D84" s="60"/>
+      <c r="E84" s="60"/>
+      <c r="F84" s="60"/>
+      <c r="G84" s="60"/>
+      <c r="H84" s="60"/>
+      <c r="I84" s="60"/>
+      <c r="J84" s="60"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="9"/>
+      <c r="B85" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E85" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="9"/>
-      <c r="J84" s="9"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="61" t="s">
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="B85" s="61"/>
-      <c r="C85" s="61"/>
-      <c r="D85" s="61"/>
-      <c r="E85" s="61"/>
-      <c r="F85" s="61"/>
-      <c r="G85" s="61"/>
-      <c r="H85" s="61"/>
-      <c r="I85" s="61"/>
-      <c r="J85" s="61"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="9"/>
-      <c r="J86" s="9"/>
+      <c r="B86" s="60"/>
+      <c r="C86" s="60"/>
+      <c r="D86" s="60"/>
+      <c r="E86" s="60"/>
+      <c r="F86" s="60"/>
+      <c r="G86" s="60"/>
+      <c r="H86" s="60"/>
+      <c r="I86" s="60"/>
+      <c r="J86" s="60"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="I87" s="4"/>
-      <c r="J87" s="7"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I88" s="4"/>
+      <c r="J88" s="7"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B89" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C89" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D88" s="9" t="s">
+      <c r="D89" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E89" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F88" s="9" t="s">
+      <c r="F89" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G88" s="4" t="s">
+      <c r="G89" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H88" s="9" t="s">
+      <c r="H89" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="I88" s="9"/>
-      <c r="J88" s="9"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="64" t="s">
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B89" s="64"/>
-      <c r="C89" s="64"/>
-      <c r="D89" s="64"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
-      <c r="I89" s="7"/>
-      <c r="J89" s="7"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="61" t="s">
+      <c r="B90" s="63"/>
+      <c r="C90" s="63"/>
+      <c r="D90" s="63"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B90" s="61"/>
-      <c r="C90" s="61"/>
-      <c r="D90" s="61"/>
-      <c r="E90" s="61"/>
-      <c r="F90" s="61"/>
-      <c r="G90" s="61"/>
-      <c r="H90" s="61"/>
-      <c r="I90" s="61"/>
-      <c r="J90" s="61"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D91" s="51" t="s">
-        <v>180</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H91" s="51" t="s">
-        <v>182</v>
-      </c>
-      <c r="I91" s="3"/>
-      <c r="J91" s="7"/>
+      <c r="B91" s="60"/>
+      <c r="C91" s="60"/>
+      <c r="D91" s="60"/>
+      <c r="E91" s="60"/>
+      <c r="F91" s="60"/>
+      <c r="G91" s="60"/>
+      <c r="H91" s="60"/>
+      <c r="I91" s="60"/>
+      <c r="J91" s="60"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D92" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H92" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="7"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B92" s="52" t="s">
+      <c r="B93" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C93" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D92" s="52" t="s">
+      <c r="D93" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="E93" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F92" s="52" t="s">
+      <c r="F93" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="G92" s="4" t="s">
+      <c r="G93" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="H92" s="52" t="s">
+      <c r="H93" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="I92" s="9"/>
-      <c r="J92" s="9"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="61" t="s">
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="B93" s="61"/>
-      <c r="C93" s="61"/>
-      <c r="D93" s="61"/>
-      <c r="E93" s="61"/>
-      <c r="F93" s="61"/>
-      <c r="G93" s="61"/>
-      <c r="H93" s="61"/>
-      <c r="I93" s="61"/>
-      <c r="J93" s="61"/>
-    </row>
-    <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="7"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-    </row>
-    <row r="95" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B95" s="53" t="s">
-        <v>187</v>
-      </c>
-      <c r="C95" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="6"/>
+      <c r="B94" s="60"/>
+      <c r="C94" s="60"/>
+      <c r="D94" s="60"/>
+      <c r="E94" s="60"/>
+      <c r="F94" s="60"/>
+      <c r="G94" s="60"/>
+      <c r="H94" s="60"/>
+      <c r="I94" s="60"/>
+      <c r="J94" s="60"/>
+    </row>
+    <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="7"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
+    <row r="96" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B96" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="C96" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="6"/>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
     </row>
-    <row r="97" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="54" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="17"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+    </row>
+    <row r="98" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="B97" s="54"/>
-      <c r="C97" s="54"/>
-      <c r="D97" s="54"/>
-      <c r="E97" s="54"/>
-      <c r="F97" s="54"/>
-      <c r="G97" s="54"/>
-      <c r="H97" s="54"/>
-      <c r="I97" s="9"/>
-      <c r="J97" s="9"/>
-    </row>
-    <row r="98" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="65" t="s">
+      <c r="B98" s="53"/>
+      <c r="C98" s="53"/>
+      <c r="D98" s="53"/>
+      <c r="E98" s="53"/>
+      <c r="F98" s="53"/>
+      <c r="G98" s="53"/>
+      <c r="H98" s="53"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+    </row>
+    <row r="99" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="B98" s="65"/>
-      <c r="C98" s="65"/>
-      <c r="D98" s="65"/>
-      <c r="E98" s="65"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="8"/>
-      <c r="J98" s="8"/>
-    </row>
-    <row r="99" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="37" t="s">
+      <c r="B99" s="64"/>
+      <c r="C99" s="64"/>
+      <c r="D99" s="64"/>
+      <c r="E99" s="64"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+    </row>
+    <row r="100" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="B99" s="38" t="s">
+      <c r="B100" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="9"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="9"/>
-      <c r="J99" s="9"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
@@ -8626,69 +8687,69 @@
       <c r="J100" s="9"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="B101" s="74"/>
-      <c r="C101" s="74"/>
-      <c r="D101" s="74"/>
-      <c r="E101" s="74"/>
-      <c r="F101" s="74"/>
-      <c r="G101" s="74"/>
-      <c r="H101" s="74"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
       <c r="I101" s="9"/>
       <c r="J101" s="9"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="9"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="9"/>
+      <c r="A102" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="B102" s="73"/>
+      <c r="C102" s="73"/>
+      <c r="D102" s="73"/>
+      <c r="E102" s="73"/>
+      <c r="F102" s="73"/>
+      <c r="G102" s="73"/>
+      <c r="H102" s="73"/>
       <c r="I102" s="9"/>
       <c r="J102" s="9"/>
     </row>
-    <row r="103" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="64" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+    </row>
+    <row r="104" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="B103" s="64"/>
-      <c r="C103" s="64"/>
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
-      <c r="F103" s="7"/>
-      <c r="G103" s="7"/>
-      <c r="H103" s="7"/>
-      <c r="I103" s="7"/>
-      <c r="J103" s="7"/>
-    </row>
-    <row r="104" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C104" s="54" t="s">
-        <v>122</v>
-      </c>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
+      <c r="B104" s="63"/>
+      <c r="C104" s="63"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="7"/>
-      <c r="B105" s="17"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
+    <row r="105" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C105" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
@@ -8696,44 +8757,38 @@
       <c r="J105" s="7"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="74" t="s">
-        <v>123</v>
-      </c>
-      <c r="B106" s="74"/>
-      <c r="C106" s="74"/>
-      <c r="D106" s="74"/>
-      <c r="E106" s="74"/>
+      <c r="A106" s="7"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
     </row>
-    <row r="107" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="64" t="s">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="B107" s="73"/>
+      <c r="C107" s="73"/>
+      <c r="D107" s="73"/>
+      <c r="E107" s="73"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+    </row>
+    <row r="108" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="B107" s="64"/>
-      <c r="C107" s="64"/>
-      <c r="D107" s="64"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="9"/>
-      <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-    </row>
-    <row r="108" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B108" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="C108" s="54" t="s">
-        <v>122</v>
-      </c>
-      <c r="D108" s="9"/>
+      <c r="B108" s="63"/>
+      <c r="C108" s="63"/>
+      <c r="D108" s="63"/>
       <c r="E108" s="9"/>
       <c r="F108" s="9"/>
       <c r="G108" s="9"/>
@@ -8741,10 +8796,16 @@
       <c r="I108" s="9"/>
       <c r="J108" s="9"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="9"/>
-      <c r="B109" s="9"/>
-      <c r="C109" s="9"/>
+    <row r="109" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C109" s="53" t="s">
+        <v>122</v>
+      </c>
       <c r="D109" s="9"/>
       <c r="E109" s="9"/>
       <c r="F109" s="9"/>
@@ -8754,86 +8815,99 @@
       <c r="J109" s="9"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="74" t="s">
+      <c r="A110" s="9"/>
+      <c r="B110" s="9"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="9"/>
+      <c r="J110" s="9"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="B110" s="74"/>
-      <c r="C110" s="74"/>
-      <c r="D110" s="74"/>
-      <c r="E110" s="74"/>
-      <c r="F110" s="74"/>
-      <c r="G110" s="74"/>
-      <c r="H110" s="74"/>
-      <c r="I110" s="74"/>
-      <c r="J110" s="9"/>
-    </row>
-    <row r="111" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="9"/>
-      <c r="B111" s="9"/>
-      <c r="C111" s="9"/>
-      <c r="D111" s="9"/>
-      <c r="E111" s="9"/>
-      <c r="F111" s="9"/>
-      <c r="G111" s="9"/>
-      <c r="H111" s="9"/>
-      <c r="I111" s="9"/>
+      <c r="B111" s="73"/>
+      <c r="C111" s="73"/>
+      <c r="D111" s="73"/>
+      <c r="E111" s="73"/>
+      <c r="F111" s="73"/>
+      <c r="G111" s="73"/>
+      <c r="H111" s="73"/>
+      <c r="I111" s="73"/>
       <c r="J111" s="9"/>
     </row>
-    <row r="112" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="B112" s="65"/>
-      <c r="C112" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D112" s="55" t="s">
-        <v>191</v>
-      </c>
-      <c r="E112" s="56" t="s">
-        <v>129</v>
-      </c>
+    <row r="112" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
       <c r="F112" s="9"/>
       <c r="G112" s="9"/>
       <c r="H112" s="9"/>
       <c r="I112" s="9"/>
       <c r="J112" s="9"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="9"/>
-      <c r="B113" s="9"/>
-      <c r="C113" s="9"/>
-      <c r="D113" s="9"/>
-      <c r="E113" s="9"/>
+    <row r="113" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="B113" s="64"/>
+      <c r="C113" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="D113" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="E113" s="55" t="s">
+        <v>129</v>
+      </c>
       <c r="F113" s="9"/>
       <c r="G113" s="9"/>
       <c r="H113" s="9"/>
       <c r="I113" s="9"/>
       <c r="J113" s="9"/>
     </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="9"/>
+      <c r="B114" s="9"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+      <c r="G114" s="9"/>
+      <c r="H114" s="9"/>
+      <c r="I114" s="9"/>
+      <c r="J114" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="A106:E106"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A110:I110"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A90:J90"/>
-    <mergeCell ref="A93:J93"/>
-    <mergeCell ref="A98:E98"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="A103:C103"/>
-    <mergeCell ref="A85:J85"/>
+  <mergeCells count="60">
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A111:I111"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="A94:J94"/>
+    <mergeCell ref="A99:E99"/>
+    <mergeCell ref="A102:H102"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="A86:J86"/>
     <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="A67:J67"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A78:J78"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="A83:J83"/>
+    <mergeCell ref="A66:J66"/>
+    <mergeCell ref="A68:J68"/>
+    <mergeCell ref="A70:J70"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A79:J79"/>
+    <mergeCell ref="A81:F81"/>
+    <mergeCell ref="A82:J82"/>
+    <mergeCell ref="A84:J84"/>
+    <mergeCell ref="B65:G65"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="A47:J47"/>
     <mergeCell ref="B48:F48"/>

</xml_diff>